<commit_message>
updated own use and losses labels
</commit_message>
<xml_diff>
--- a/config/9th_EBT_schema.xlsx
+++ b/config/9th_EBT_schema.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\APERC\transport_model_9th_edition\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hyuga.kasai\Documents\Github\9th_Visualization\9th_edition_visualisation\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EB54108-0B61-467D-856C-8F7BB1D66EA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88D6D4A2-F86A-412C-9D7B-11581317FCFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{F61A5A6E-F35F-447D-A8FA-A636DA54EBA1}"/>
+    <workbookView xWindow="-6750" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{F61A5A6E-F35F-447D-A8FA-A636DA54EBA1}"/>
   </bookViews>
   <sheets>
     <sheet name="9th_EBT_schema" sheetId="1" r:id="rId1"/>
@@ -546,9 +546,6 @@
     <t>18_electricity_output_in_gwh</t>
   </si>
   <si>
-    <t>10_02_transmision_and_distribution_losses</t>
-  </si>
-  <si>
     <t>09_x_02_gas</t>
   </si>
   <si>
@@ -876,9 +873,6 @@
     <t>19_02_heat_plants</t>
   </si>
   <si>
-    <t>10_01_05_natural_gas_blending_plants</t>
-  </si>
-  <si>
     <t>18_01_02_02_combinedcycle</t>
   </si>
   <si>
@@ -888,102 +882,66 @@
     <t>x</t>
   </si>
   <si>
-    <t>10_01_08_coke_ovens</t>
-  </si>
-  <si>
     <t>18_01_02_03_ccs</t>
   </si>
   <si>
     <t>15_02_02_03_03_battery_ev</t>
   </si>
   <si>
-    <t>10_01_09_coal_mines</t>
-  </si>
-  <si>
     <t>18_01_05_01_large</t>
   </si>
   <si>
     <t>15_02_02_03_04_compressed_natual_gas</t>
   </si>
   <si>
-    <t>10_01_10_blast_furnaces</t>
-  </si>
-  <si>
     <t>18_01_05_02_mediumsmall</t>
   </si>
   <si>
     <t>15_02_02_03_05_plugin_hybrid_ev_gasoline</t>
   </si>
   <si>
-    <t>10_01_14_oil_refineries</t>
-  </si>
-  <si>
     <t>18_01_05_03_pump</t>
   </si>
   <si>
     <t>15_02_02_03_06_plugin_hybrid_ev_diesel</t>
   </si>
   <si>
-    <t>10_01_15_oil_and_gas_extraction</t>
-  </si>
-  <si>
     <t>18_01_08_01_utility</t>
   </si>
   <si>
     <t>15_02_02_04_01_diesel_engine</t>
   </si>
   <si>
-    <t>10_01_16_biofuels_processing</t>
-  </si>
-  <si>
     <t>18_01_08_02_rooftop</t>
   </si>
   <si>
     <t>15_02_02_04_02_gasoline_engine</t>
   </si>
   <si>
-    <t>10_01_19_ccs</t>
-  </si>
-  <si>
     <t>18_01_08_03_csp</t>
   </si>
   <si>
     <t>15_02_02_04_03_battery_ev</t>
   </si>
   <si>
-    <t>10_01_07_gas_separation</t>
-  </si>
-  <si>
     <t>18_01_09_01_onshore</t>
   </si>
   <si>
     <t>15_02_02_04_04_compressed_natual_gas</t>
   </si>
   <si>
-    <t>10_01_06_gastoliquids_plants</t>
-  </si>
-  <si>
     <t>18_01_09_02_offshore</t>
   </si>
   <si>
     <t>15_02_02_04_05_plugin_hybrid_ev_gasoline</t>
   </si>
   <si>
-    <t>10_01_12_bkb_pb_plants</t>
-  </si>
-  <si>
     <t>15_02_02_04_06_plugin_hybrid_ev_diesel</t>
   </si>
   <si>
-    <t>10_01_18_nonspecified_own_uses</t>
-  </si>
-  <si>
     <t>10_01_02_gas_works_plants</t>
   </si>
   <si>
-    <t>10_01_13_liquefaction_plants_coal_to_oil</t>
-  </si>
-  <si>
     <t>14_03_01_iron_and_steel</t>
   </si>
   <si>
@@ -1216,13 +1174,55 @@
   </si>
   <si>
     <t>15_02_01_01_08_fuel_cell_ev</t>
+  </si>
+  <si>
+    <t>10_01_13_pump_storage_plants</t>
+  </si>
+  <si>
+    <t>10_01_05_coke_ovens</t>
+  </si>
+  <si>
+    <t>10_01_06_coal_mines</t>
+  </si>
+  <si>
+    <t>10_01_07_blast_furnaces</t>
+  </si>
+  <si>
+    <t>10_01_11_oil_refineries</t>
+  </si>
+  <si>
+    <t>10_01_12_oil_and_gas_extraction</t>
+  </si>
+  <si>
+    <t>10_01_15_charcoal_production_plants</t>
+  </si>
+  <si>
+    <t>10_01_18_ccs</t>
+  </si>
+  <si>
+    <t>10_01_16_gasification_plants_for_biogases</t>
+  </si>
+  <si>
+    <t>10_01_04_gastoliquids_plants</t>
+  </si>
+  <si>
+    <t>10_01_09_bkb_pb_plants</t>
+  </si>
+  <si>
+    <t>10_01_17_nonspecified_own_uses</t>
+  </si>
+  <si>
+    <t>10_01_10_liquefaction_plants_coal_to_oil</t>
+  </si>
+  <si>
+    <t>10_02_transmission_and_distribution_losses</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1245,12 +1245,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -1661,29 +1655,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CCBC1CD-CC2F-455C-8B9B-5A132B98DEED}">
   <dimension ref="A1:I102"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K71" sqref="K71"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A14" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.77734375" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="42.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="45.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="41.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="42.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="45.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="41.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="41" customWidth="1"/>
-    <col min="9" max="9" width="40.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="40.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -1712,7 +1706,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1741,7 +1735,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -1770,7 +1764,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>28</v>
       </c>
@@ -1796,7 +1790,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>36</v>
       </c>
@@ -1822,7 +1816,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>44</v>
       </c>
@@ -1848,7 +1842,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>52</v>
       </c>
@@ -1874,7 +1868,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>60</v>
       </c>
@@ -1900,7 +1894,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>68</v>
       </c>
@@ -1926,7 +1920,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>76</v>
       </c>
@@ -1952,7 +1946,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>84</v>
       </c>
@@ -1978,7 +1972,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>92</v>
       </c>
@@ -2004,7 +1998,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>100</v>
       </c>
@@ -2030,7 +2024,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>108</v>
       </c>
@@ -2056,7 +2050,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>116</v>
       </c>
@@ -2082,7 +2076,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>124</v>
       </c>
@@ -2108,7 +2102,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>132</v>
       </c>
@@ -2134,7 +2128,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>140</v>
       </c>
@@ -2160,7 +2154,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>148</v>
       </c>
@@ -2174,850 +2168,850 @@
         <v>151</v>
       </c>
       <c r="F21" t="s">
+        <v>375</v>
+      </c>
+      <c r="G21" t="s">
         <v>152</v>
       </c>
-      <c r="G21" t="s">
+      <c r="H21" t="s">
         <v>153</v>
       </c>
-      <c r="H21" t="s">
+      <c r="I21" t="s">
         <v>154</v>
       </c>
-      <c r="I21" t="s">
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>156</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>157</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>158</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>159</v>
       </c>
-      <c r="F22" t="s">
+      <c r="G22" t="s">
         <v>160</v>
       </c>
-      <c r="G22" t="s">
+      <c r="H22" t="s">
         <v>161</v>
       </c>
-      <c r="H22" t="s">
+      <c r="I22" t="s">
         <v>162</v>
       </c>
-      <c r="I22" t="s">
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>164</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>165</v>
       </c>
-      <c r="D23" t="s">
+      <c r="F23" t="s">
         <v>166</v>
       </c>
-      <c r="F23" t="s">
+      <c r="G23" t="s">
         <v>167</v>
       </c>
-      <c r="G23" t="s">
+      <c r="H23" t="s">
         <v>168</v>
       </c>
-      <c r="H23" t="s">
+      <c r="I23" t="s">
         <v>169</v>
       </c>
-      <c r="I23" t="s">
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>171</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>172</v>
       </c>
-      <c r="D24" t="s">
+      <c r="F24" t="s">
         <v>173</v>
       </c>
-      <c r="F24" t="s">
+      <c r="G24" t="s">
         <v>174</v>
       </c>
-      <c r="G24" t="s">
+      <c r="H24" t="s">
         <v>175</v>
       </c>
-      <c r="H24" t="s">
+      <c r="I24" t="s">
         <v>176</v>
       </c>
-      <c r="I24" t="s">
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B25" t="s">
+      <c r="D25" t="s">
         <v>178</v>
       </c>
-      <c r="D25" t="s">
+      <c r="F25" t="s">
         <v>179</v>
       </c>
-      <c r="F25" t="s">
+      <c r="G25" t="s">
         <v>180</v>
       </c>
-      <c r="G25" t="s">
+      <c r="H25" t="s">
         <v>181</v>
       </c>
-      <c r="H25" t="s">
+      <c r="I25" t="s">
         <v>182</v>
       </c>
-      <c r="I25" t="s">
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B26" t="s">
+      <c r="D26" t="s">
         <v>184</v>
       </c>
-      <c r="D26" t="s">
+      <c r="F26" t="s">
         <v>185</v>
       </c>
-      <c r="F26" t="s">
+      <c r="G26" t="s">
         <v>186</v>
       </c>
-      <c r="G26" t="s">
+      <c r="H26" t="s">
         <v>187</v>
       </c>
-      <c r="H26" t="s">
+      <c r="I26" t="s">
         <v>188</v>
       </c>
-      <c r="I26" t="s">
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B27" t="s">
+      <c r="D27" t="s">
         <v>190</v>
       </c>
-      <c r="D27" t="s">
+      <c r="F27" t="s">
         <v>191</v>
       </c>
-      <c r="F27" t="s">
+      <c r="G27" t="s">
         <v>192</v>
       </c>
-      <c r="G27" t="s">
+      <c r="H27" t="s">
         <v>193</v>
       </c>
-      <c r="H27" t="s">
+      <c r="I27" t="s">
         <v>194</v>
       </c>
-      <c r="I27" t="s">
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B28" t="s">
+      <c r="D28" t="s">
         <v>196</v>
       </c>
-      <c r="D28" t="s">
+      <c r="F28" t="s">
         <v>197</v>
       </c>
-      <c r="F28" t="s">
+      <c r="G28" t="s">
         <v>198</v>
       </c>
-      <c r="G28" t="s">
+      <c r="H28" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="H28" s="6" t="s">
+      <c r="I28" t="s">
         <v>200</v>
       </c>
-      <c r="I28" t="s">
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B29" t="s">
+      <c r="D29" t="s">
         <v>202</v>
       </c>
-      <c r="D29" t="s">
+      <c r="F29" t="s">
         <v>203</v>
       </c>
-      <c r="F29" t="s">
+      <c r="G29" t="s">
         <v>204</v>
       </c>
-      <c r="G29" t="s">
+      <c r="H29" s="6" t="s">
+        <v>343</v>
+      </c>
+      <c r="I29" t="s">
         <v>205</v>
       </c>
-      <c r="H29" s="6" t="s">
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>206</v>
+      </c>
+      <c r="D30" t="s">
+        <v>207</v>
+      </c>
+      <c r="F30" t="s">
+        <v>208</v>
+      </c>
+      <c r="G30" t="s">
+        <v>209</v>
+      </c>
+      <c r="H30" s="6" t="s">
+        <v>342</v>
+      </c>
+      <c r="I30" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>211</v>
+      </c>
+      <c r="D31" t="s">
+        <v>212</v>
+      </c>
+      <c r="F31" t="s">
+        <v>213</v>
+      </c>
+      <c r="G31" t="s">
+        <v>214</v>
+      </c>
+      <c r="H31" s="6" t="s">
+        <v>341</v>
+      </c>
+      <c r="I31" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D32" t="s">
+        <v>216</v>
+      </c>
+      <c r="F32" t="s">
+        <v>217</v>
+      </c>
+      <c r="G32" t="s">
+        <v>218</v>
+      </c>
+      <c r="H32" s="6" t="s">
+        <v>344</v>
+      </c>
+      <c r="I32" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="33" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D33" t="s">
+        <v>221</v>
+      </c>
+      <c r="F33" t="s">
+        <v>222</v>
+      </c>
+      <c r="G33" t="s">
+        <v>223</v>
+      </c>
+      <c r="H33" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="I33" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="34" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D34" t="s">
+        <v>225</v>
+      </c>
+      <c r="F34" t="s">
+        <v>226</v>
+      </c>
+      <c r="G34" t="s">
+        <v>227</v>
+      </c>
+      <c r="H34" s="6" t="s">
+        <v>339</v>
+      </c>
+      <c r="I34" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="35" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D35" t="s">
+        <v>229</v>
+      </c>
+      <c r="F35" t="s">
+        <v>230</v>
+      </c>
+      <c r="G35" t="s">
+        <v>231</v>
+      </c>
+      <c r="H35" s="6" t="s">
+        <v>340</v>
+      </c>
+      <c r="I35" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="36" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D36" t="s">
+        <v>234</v>
+      </c>
+      <c r="F36" t="s">
+        <v>235</v>
+      </c>
+      <c r="G36" t="s">
+        <v>236</v>
+      </c>
+      <c r="H36" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="I36" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="37" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D37" t="s">
+        <v>239</v>
+      </c>
+      <c r="F37" t="s">
+        <v>240</v>
+      </c>
+      <c r="G37" t="s">
+        <v>241</v>
+      </c>
+      <c r="H37" t="s">
+        <v>237</v>
+      </c>
+      <c r="I37" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="38" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D38" t="s">
+        <v>244</v>
+      </c>
+      <c r="F38" t="s">
+        <v>245</v>
+      </c>
+      <c r="G38" t="s">
+        <v>246</v>
+      </c>
+      <c r="H38" t="s">
+        <v>242</v>
+      </c>
+      <c r="I38" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="39" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D39" t="s">
+        <v>249</v>
+      </c>
+      <c r="F39" t="s">
+        <v>250</v>
+      </c>
+      <c r="G39" t="s">
+        <v>251</v>
+      </c>
+      <c r="H39" t="s">
+        <v>247</v>
+      </c>
+      <c r="I39" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="40" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D40" t="s">
+        <v>254</v>
+      </c>
+      <c r="F40" t="s">
+        <v>255</v>
+      </c>
+      <c r="G40" t="s">
+        <v>256</v>
+      </c>
+      <c r="H40" t="s">
+        <v>252</v>
+      </c>
+      <c r="I40" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="41" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D41" t="s">
+        <v>259</v>
+      </c>
+      <c r="F41" t="s">
+        <v>260</v>
+      </c>
+      <c r="G41" t="s">
+        <v>362</v>
+      </c>
+      <c r="H41" t="s">
+        <v>257</v>
+      </c>
+      <c r="I41" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="42" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D42" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="F42" t="s">
+        <v>263</v>
+      </c>
+      <c r="G42" t="s">
+        <v>363</v>
+      </c>
+      <c r="H42" t="s">
+        <v>261</v>
+      </c>
+      <c r="I42" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="43" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D43" t="s">
+        <v>263</v>
+      </c>
+      <c r="G43" t="s">
+        <v>364</v>
+      </c>
+      <c r="H43" t="s">
+        <v>264</v>
+      </c>
+      <c r="I43" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="44" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="G44" t="s">
+        <v>365</v>
+      </c>
+      <c r="H44" t="s">
+        <v>266</v>
+      </c>
+      <c r="I44" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="45" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="G45" t="s">
+        <v>366</v>
+      </c>
+      <c r="H45" t="s">
+        <v>268</v>
+      </c>
+      <c r="I45" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="46" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="G46" t="s">
+        <v>367</v>
+      </c>
+      <c r="H46" t="s">
+        <v>270</v>
+      </c>
+      <c r="I46" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="47" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="G47" t="s">
+        <v>368</v>
+      </c>
+      <c r="H47" t="s">
+        <v>272</v>
+      </c>
+      <c r="I47" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="48" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="G48" t="s">
+        <v>369</v>
+      </c>
+      <c r="H48" t="s">
+        <v>274</v>
+      </c>
+      <c r="I48" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="49" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G49" t="s">
+        <v>370</v>
+      </c>
+      <c r="H49" t="s">
+        <v>276</v>
+      </c>
+      <c r="I49" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="50" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G50" t="s">
+        <v>371</v>
+      </c>
+      <c r="H50" t="s">
+        <v>278</v>
+      </c>
+      <c r="I50" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="51" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G51" t="s">
+        <v>372</v>
+      </c>
+      <c r="H51" t="s">
+        <v>280</v>
+      </c>
+      <c r="I51" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="52" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G52" t="s">
+        <v>373</v>
+      </c>
+      <c r="H52" t="s">
+        <v>263</v>
+      </c>
+      <c r="I52" s="5" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="53" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G53" t="s">
+        <v>283</v>
+      </c>
+      <c r="I53" s="5" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="54" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G54" t="s">
+        <v>374</v>
+      </c>
+      <c r="H54" s="7" t="s">
+        <v>346</v>
+      </c>
+      <c r="I54" s="5" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="55" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G55" t="s">
+        <v>284</v>
+      </c>
+      <c r="I55" s="5" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="56" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G56" t="s">
+        <v>285</v>
+      </c>
+      <c r="I56" s="5" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="57" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G57" t="s">
+        <v>286</v>
+      </c>
+      <c r="I57" s="5" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="58" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G58" t="s">
+        <v>287</v>
+      </c>
+      <c r="I58" s="5" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="59" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G59" t="s">
+        <v>288</v>
+      </c>
+      <c r="I59" s="5" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="60" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G60" t="s">
+        <v>289</v>
+      </c>
+      <c r="I60" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="61" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G61" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="62" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G62" t="s">
+        <v>291</v>
+      </c>
+      <c r="I62" s="7" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="63" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G63" t="s">
+        <v>292</v>
+      </c>
+      <c r="I63" s="7" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="64" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G64" t="s">
+        <v>293</v>
+      </c>
+      <c r="I64" s="7" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="65" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G65" t="s">
+        <v>294</v>
+      </c>
+      <c r="I65" s="7" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="66" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G66" t="s">
+        <v>295</v>
+      </c>
+      <c r="I66" s="7" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="67" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G67" t="s">
+        <v>296</v>
+      </c>
+      <c r="I67" s="7" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="68" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G68" t="s">
+        <v>297</v>
+      </c>
+      <c r="I68" s="7" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="69" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G69" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="70" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G70" t="s">
+        <v>299</v>
+      </c>
+      <c r="I70" s="7" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="71" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G71" t="s">
+        <v>300</v>
+      </c>
+      <c r="I71" s="7" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="72" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G72" t="s">
+        <v>301</v>
+      </c>
+      <c r="I72" s="7" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="73" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G73" t="s">
+        <v>302</v>
+      </c>
+      <c r="I73" s="7" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="74" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G74" t="s">
+        <v>303</v>
+      </c>
+      <c r="I74" s="7" t="s">
         <v>357</v>
       </c>
-      <c r="I29" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B30" t="s">
-        <v>207</v>
-      </c>
-      <c r="D30" t="s">
-        <v>208</v>
-      </c>
-      <c r="F30" t="s">
-        <v>209</v>
-      </c>
-      <c r="G30" t="s">
-        <v>210</v>
-      </c>
-      <c r="H30" s="6" t="s">
-        <v>356</v>
-      </c>
-      <c r="I30" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B31" t="s">
-        <v>212</v>
-      </c>
-      <c r="D31" t="s">
-        <v>213</v>
-      </c>
-      <c r="F31" t="s">
-        <v>214</v>
-      </c>
-      <c r="G31" t="s">
-        <v>215</v>
-      </c>
-      <c r="H31" s="6" t="s">
-        <v>355</v>
-      </c>
-      <c r="I31" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D32" t="s">
-        <v>217</v>
-      </c>
-      <c r="F32" t="s">
-        <v>218</v>
-      </c>
-      <c r="G32" t="s">
-        <v>219</v>
-      </c>
-      <c r="H32" s="6" t="s">
+    </row>
+    <row r="75" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G75" t="s">
+        <v>304</v>
+      </c>
+      <c r="I75" s="7" t="s">
         <v>358</v>
       </c>
-      <c r="I32" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="33" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D33" t="s">
-        <v>222</v>
-      </c>
-      <c r="F33" t="s">
-        <v>223</v>
-      </c>
-      <c r="G33" t="s">
-        <v>224</v>
-      </c>
-      <c r="H33" s="6" t="s">
-        <v>220</v>
-      </c>
-      <c r="I33" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="34" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D34" t="s">
-        <v>226</v>
-      </c>
-      <c r="F34" t="s">
-        <v>227</v>
-      </c>
-      <c r="G34" t="s">
-        <v>228</v>
-      </c>
-      <c r="H34" s="6" t="s">
-        <v>353</v>
-      </c>
-      <c r="I34" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="35" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D35" t="s">
-        <v>230</v>
-      </c>
-      <c r="F35" t="s">
-        <v>231</v>
-      </c>
-      <c r="G35" t="s">
-        <v>232</v>
-      </c>
-      <c r="H35" s="6" t="s">
-        <v>354</v>
-      </c>
-      <c r="I35" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="36" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D36" t="s">
-        <v>235</v>
-      </c>
-      <c r="F36" t="s">
-        <v>236</v>
-      </c>
-      <c r="G36" t="s">
-        <v>237</v>
-      </c>
-      <c r="H36" s="6" t="s">
-        <v>233</v>
-      </c>
-      <c r="I36" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="37" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D37" t="s">
-        <v>240</v>
-      </c>
-      <c r="F37" t="s">
-        <v>241</v>
-      </c>
-      <c r="G37" t="s">
-        <v>242</v>
-      </c>
-      <c r="H37" t="s">
-        <v>238</v>
-      </c>
-      <c r="I37" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="38" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D38" t="s">
-        <v>245</v>
-      </c>
-      <c r="F38" t="s">
-        <v>246</v>
-      </c>
-      <c r="G38" t="s">
-        <v>247</v>
-      </c>
-      <c r="H38" t="s">
-        <v>243</v>
-      </c>
-      <c r="I38" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="39" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D39" t="s">
-        <v>250</v>
-      </c>
-      <c r="F39" t="s">
-        <v>251</v>
-      </c>
-      <c r="G39" t="s">
-        <v>252</v>
-      </c>
-      <c r="H39" t="s">
-        <v>248</v>
-      </c>
-      <c r="I39" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="40" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D40" t="s">
-        <v>255</v>
-      </c>
-      <c r="F40" t="s">
-        <v>256</v>
-      </c>
-      <c r="G40" t="s">
-        <v>257</v>
-      </c>
-      <c r="H40" t="s">
-        <v>253</v>
-      </c>
-      <c r="I40" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="41" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D41" t="s">
-        <v>260</v>
-      </c>
-      <c r="F41" t="s">
-        <v>261</v>
-      </c>
-      <c r="G41" t="s">
-        <v>262</v>
-      </c>
-      <c r="H41" t="s">
-        <v>258</v>
-      </c>
-      <c r="I41" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="42" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D42" s="5" t="s">
+    </row>
+    <row r="76" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G76" t="s">
+        <v>305</v>
+      </c>
+      <c r="I76" s="7" t="s">
         <v>359</v>
       </c>
-      <c r="F42" t="s">
-        <v>265</v>
-      </c>
-      <c r="G42" t="s">
-        <v>266</v>
-      </c>
-      <c r="H42" t="s">
+    </row>
+    <row r="77" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G77" t="s">
+        <v>306</v>
+      </c>
+      <c r="I77" s="7" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="78" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G78" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="79" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G79" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="80" spans="7:9" x14ac:dyDescent="0.25">
+      <c r="G80" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="81" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G81" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="82" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G82" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="83" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G83" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="84" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G84" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="85" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G85" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="86" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G86" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="87" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G87" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="88" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G88" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="89" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G89" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="90" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G90" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="91" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G91" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="92" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G92" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="93" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G93" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="94" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G94" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="95" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G95" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="96" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G96" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="97" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G97" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="98" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G98" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="99" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G99" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="100" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G100" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="101" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G101" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="102" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G102" t="s">
         <v>263</v>
-      </c>
-      <c r="I42" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="43" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D43" t="s">
-        <v>265</v>
-      </c>
-      <c r="G43" t="s">
-        <v>269</v>
-      </c>
-      <c r="H43" t="s">
-        <v>267</v>
-      </c>
-      <c r="I43" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="44" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="G44" t="s">
-        <v>272</v>
-      </c>
-      <c r="H44" t="s">
-        <v>270</v>
-      </c>
-      <c r="I44" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="45" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="G45" t="s">
-        <v>275</v>
-      </c>
-      <c r="H45" t="s">
-        <v>273</v>
-      </c>
-      <c r="I45" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="46" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="G46" t="s">
-        <v>278</v>
-      </c>
-      <c r="H46" t="s">
-        <v>276</v>
-      </c>
-      <c r="I46" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="47" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="G47" t="s">
-        <v>281</v>
-      </c>
-      <c r="H47" t="s">
-        <v>279</v>
-      </c>
-      <c r="I47" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="48" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="G48" t="s">
-        <v>284</v>
-      </c>
-      <c r="H48" t="s">
-        <v>282</v>
-      </c>
-      <c r="I48" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="49" spans="7:9" x14ac:dyDescent="0.3">
-      <c r="G49" t="s">
-        <v>287</v>
-      </c>
-      <c r="H49" t="s">
-        <v>285</v>
-      </c>
-      <c r="I49" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="50" spans="7:9" x14ac:dyDescent="0.3">
-      <c r="G50" t="s">
-        <v>290</v>
-      </c>
-      <c r="H50" t="s">
-        <v>288</v>
-      </c>
-      <c r="I50" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="51" spans="7:9" x14ac:dyDescent="0.3">
-      <c r="G51" t="s">
-        <v>293</v>
-      </c>
-      <c r="H51" t="s">
-        <v>291</v>
-      </c>
-      <c r="I51" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="52" spans="7:9" x14ac:dyDescent="0.3">
-      <c r="G52" t="s">
-        <v>295</v>
-      </c>
-      <c r="H52" t="s">
-        <v>265</v>
-      </c>
-      <c r="I52" s="5" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="53" spans="7:9" x14ac:dyDescent="0.3">
-      <c r="G53" t="s">
-        <v>296</v>
-      </c>
-      <c r="I53" s="5" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="54" spans="7:9" x14ac:dyDescent="0.3">
-      <c r="G54" t="s">
-        <v>297</v>
-      </c>
-      <c r="H54" s="7" t="s">
-        <v>360</v>
-      </c>
-      <c r="I54" s="5" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="55" spans="7:9" x14ac:dyDescent="0.3">
-      <c r="G55" t="s">
-        <v>298</v>
-      </c>
-      <c r="I55" s="5" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="56" spans="7:9" x14ac:dyDescent="0.3">
-      <c r="G56" t="s">
-        <v>299</v>
-      </c>
-      <c r="I56" s="5" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="57" spans="7:9" x14ac:dyDescent="0.3">
-      <c r="G57" t="s">
-        <v>300</v>
-      </c>
-      <c r="I57" s="5" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="58" spans="7:9" x14ac:dyDescent="0.3">
-      <c r="G58" t="s">
-        <v>301</v>
-      </c>
-      <c r="I58" s="5" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="59" spans="7:9" x14ac:dyDescent="0.3">
-      <c r="G59" t="s">
-        <v>302</v>
-      </c>
-      <c r="I59" s="5" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="60" spans="7:9" x14ac:dyDescent="0.3">
-      <c r="G60" t="s">
-        <v>303</v>
-      </c>
-      <c r="I60" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="61" spans="7:9" x14ac:dyDescent="0.3">
-      <c r="G61" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="62" spans="7:9" x14ac:dyDescent="0.3">
-      <c r="G62" t="s">
-        <v>305</v>
-      </c>
-      <c r="I62" s="7" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="63" spans="7:9" x14ac:dyDescent="0.3">
-      <c r="G63" t="s">
-        <v>306</v>
-      </c>
-      <c r="I63" s="7" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="64" spans="7:9" x14ac:dyDescent="0.3">
-      <c r="G64" t="s">
-        <v>307</v>
-      </c>
-      <c r="I64" s="7" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="65" spans="7:9" x14ac:dyDescent="0.3">
-      <c r="G65" t="s">
-        <v>308</v>
-      </c>
-      <c r="I65" s="7" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="66" spans="7:9" x14ac:dyDescent="0.3">
-      <c r="G66" t="s">
-        <v>309</v>
-      </c>
-      <c r="I66" s="7" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="67" spans="7:9" x14ac:dyDescent="0.3">
-      <c r="G67" t="s">
-        <v>310</v>
-      </c>
-      <c r="I67" s="7" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="68" spans="7:9" x14ac:dyDescent="0.3">
-      <c r="G68" t="s">
-        <v>311</v>
-      </c>
-      <c r="I68" s="7" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="69" spans="7:9" x14ac:dyDescent="0.3">
-      <c r="G69" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="70" spans="7:9" x14ac:dyDescent="0.3">
-      <c r="G70" t="s">
-        <v>313</v>
-      </c>
-      <c r="I70" s="7" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="71" spans="7:9" x14ac:dyDescent="0.3">
-      <c r="G71" t="s">
-        <v>314</v>
-      </c>
-      <c r="I71" s="7" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="72" spans="7:9" x14ac:dyDescent="0.3">
-      <c r="G72" t="s">
-        <v>315</v>
-      </c>
-      <c r="I72" s="7" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="73" spans="7:9" x14ac:dyDescent="0.3">
-      <c r="G73" t="s">
-        <v>316</v>
-      </c>
-      <c r="I73" s="7" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="74" spans="7:9" x14ac:dyDescent="0.3">
-      <c r="G74" t="s">
-        <v>317</v>
-      </c>
-      <c r="I74" s="7" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="75" spans="7:9" x14ac:dyDescent="0.3">
-      <c r="G75" t="s">
-        <v>318</v>
-      </c>
-      <c r="I75" s="7" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="76" spans="7:9" x14ac:dyDescent="0.3">
-      <c r="G76" t="s">
-        <v>319</v>
-      </c>
-      <c r="I76" s="7" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="77" spans="7:9" x14ac:dyDescent="0.3">
-      <c r="G77" t="s">
-        <v>320</v>
-      </c>
-      <c r="I77" s="7" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="78" spans="7:9" x14ac:dyDescent="0.3">
-      <c r="G78" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="79" spans="7:9" x14ac:dyDescent="0.3">
-      <c r="G79" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="80" spans="7:9" x14ac:dyDescent="0.3">
-      <c r="G80" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="81" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G81" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="82" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G82" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="83" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G83" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="84" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G84" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="85" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G85" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="86" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G86" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="87" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G87" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="88" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G88" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="89" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G89" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="90" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G90" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="91" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G91" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="92" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G92" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="93" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G93" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="94" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G94" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="95" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G95" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="96" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G96" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="97" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G97" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="98" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G98" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="99" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G99" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="100" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G100" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="101" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G101" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="102" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G102" t="s">
-        <v>265</v>
       </c>
     </row>
   </sheetData>

</xml_diff>